<commit_message>
Arquivos Estudos Algebra Linear
</commit_message>
<xml_diff>
--- a/linear-regression/case_conceitos.xlsx
+++ b/linear-regression/case_conceitos.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pedro\OneDrive\Documentos\projeto_cientista_dados\regressão_linear\metodo_minimos_quadrados\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pedro\OneDrive\Documentos\git\data-science\linear-regression\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1D9F801-F225-42C2-99CA-8F5F5C18A3A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2DF83AF-6E17-4774-98CA-C4A99176DDAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{52754B87-B5BE-4B0C-99A7-9B72E1243927}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{52754B87-B5BE-4B0C-99A7-9B72E1243927}"/>
   </bookViews>
   <sheets>
     <sheet name="ESTUDO" sheetId="1" r:id="rId1"/>
@@ -609,6 +609,33 @@
     <t>quanto o modelo errou pra mais ou pra menos</t>
   </si>
   <si>
+    <t>erro (y - ŷ)</t>
+  </si>
+  <si>
+    <t>erro_quadrado ((y - ŷ)^2)</t>
+  </si>
+  <si>
+    <t>horas (x)</t>
+  </si>
+  <si>
+    <t>pdl (y)</t>
+  </si>
+  <si>
+    <t>horas_x</t>
+  </si>
+  <si>
+    <t>pdl_y</t>
+  </si>
+  <si>
+    <t>previsto_y</t>
+  </si>
+  <si>
+    <t>erro</t>
+  </si>
+  <si>
+    <t>erro_quadrado</t>
+  </si>
+  <si>
     <r>
       <t xml:space="preserve">Isso mede </t>
     </r>
@@ -631,35 +658,8 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> (porque a gente não quer que erro positivo anule erro negativo)</t>
-    </r>
-  </si>
-  <si>
-    <t>erro (y - ŷ)</t>
-  </si>
-  <si>
-    <t>erro_quadrado ((y - ŷ)^2)</t>
-  </si>
-  <si>
-    <t>horas (x)</t>
-  </si>
-  <si>
-    <t>pdl (y)</t>
-  </si>
-  <si>
-    <t>horas_x</t>
-  </si>
-  <si>
-    <t>pdl_y</t>
-  </si>
-  <si>
-    <t>previsto_y</t>
-  </si>
-  <si>
-    <t>erro</t>
-  </si>
-  <si>
-    <t>erro_quadrado</t>
+      <t xml:space="preserve"> (ao quadrado porque a gente não quer que erro positivo anule erro negativo. Também queremos punir grandes erros)</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -757,9 +757,6 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -775,6 +772,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1989,15 +1989,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>2752724</xdr:colOff>
+      <xdr:colOff>2181224</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>1009650</xdr:rowOff>
+      <xdr:rowOff>981075</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>3375023</xdr:colOff>
+      <xdr:colOff>2803523</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>1276350</xdr:rowOff>
+      <xdr:rowOff>1247775</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2020,7 +2020,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="50406299" y="1200150"/>
+          <a:off x="49834799" y="1171575"/>
           <a:ext cx="622299" cy="266700"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -2393,8 +2393,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F5A3A9D-C9A5-4292-A8D0-66F0683F8F7A}">
   <dimension ref="A1:O15"/>
   <sheetViews>
-    <sheetView topLeftCell="L1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M4" sqref="M4:M8"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="O20" sqref="O20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2412,7 +2412,7 @@
     <col min="12" max="12" width="92.42578125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="96.7109375" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="43.140625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="85.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="72.140625" style="5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15">
@@ -2423,10 +2423,10 @@
         <v>0</v>
       </c>
       <c r="C1" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>43</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>44</v>
       </c>
       <c r="E1" s="4" t="s">
         <v>24</v>
@@ -2449,96 +2449,97 @@
       <c r="K1" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="L1" s="9" t="s">
+      <c r="L1" s="8" t="s">
         <v>33</v>
       </c>
       <c r="M1" s="4" t="s">
         <v>37</v>
       </c>
       <c r="N1" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="O1" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="O1" s="8" t="s">
-        <v>42</v>
-      </c>
     </row>
-    <row r="2" spans="1:15" s="7" customFormat="1" ht="111.75" customHeight="1">
-      <c r="A2" s="8" t="s">
+    <row r="2" spans="1:15" s="6" customFormat="1" ht="111.75" customHeight="1">
+      <c r="A2" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="E2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="F2" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="G2" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H2" s="6" t="s">
+      <c r="H2" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="I2" s="6" t="s">
+      <c r="I2" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="J2" s="6" t="s">
+      <c r="J2" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="K2" s="7" t="s">
+      <c r="K2" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="L2" s="7" t="s">
+      <c r="L2" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="M2" s="7" t="s">
+      <c r="M2" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="N2" s="7" t="s">
+      <c r="N2" s="6" t="s">
         <v>39</v>
       </c>
       <c r="O2" s="5" t="s">
-        <v>40</v>
+        <v>49</v>
       </c>
     </row>
-    <row r="3" spans="1:15" s="7" customFormat="1" ht="30">
-      <c r="A3" s="8" t="s">
+    <row r="3" spans="1:15" s="6" customFormat="1" ht="30">
+      <c r="A3" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B3" s="6"/>
-      <c r="C3" s="6"/>
-      <c r="D3" s="6"/>
-      <c r="E3" s="6"/>
-      <c r="F3" s="6"/>
-      <c r="G3" s="7" t="s">
+      <c r="B3" s="5"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="H3" s="6" t="s">
+      <c r="H3" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="I3" s="6" t="s">
+      <c r="I3" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="J3" s="7" t="s">
+      <c r="J3" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="K3" s="7" t="s">
+      <c r="K3" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="L3" s="7" t="s">
+      <c r="L3" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="M3" s="7" t="s">
+      <c r="M3" s="6" t="s">
         <v>38</v>
       </c>
+      <c r="O3" s="5"/>
     </row>
     <row r="4" spans="1:15">
       <c r="A4" s="3" t="s">
@@ -2593,7 +2594,7 @@
         <f>D4-M4</f>
         <v>-2</v>
       </c>
-      <c r="O4">
+      <c r="O4" s="11">
         <f>(D4-M4)^2</f>
         <v>4</v>
       </c>
@@ -2635,7 +2636,7 @@
         <f t="shared" ref="N5:N8" si="5">D5-M5</f>
         <v>1.5</v>
       </c>
-      <c r="O5">
+      <c r="O5" s="11">
         <f t="shared" ref="O5:O8" si="6">(D5-M5)^2</f>
         <v>2.25</v>
       </c>
@@ -2677,7 +2678,7 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="O6">
+      <c r="O6" s="11">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
@@ -2719,7 +2720,7 @@
         <f t="shared" si="5"/>
         <v>3.5</v>
       </c>
-      <c r="O7">
+      <c r="O7" s="11">
         <f t="shared" si="6"/>
         <v>12.25</v>
       </c>
@@ -2761,16 +2762,16 @@
         <f t="shared" si="5"/>
         <v>-3</v>
       </c>
-      <c r="O8">
+      <c r="O8" s="11">
         <f t="shared" si="6"/>
         <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:15">
-      <c r="I10" s="9" t="s">
+      <c r="I10" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="J10" s="10" t="s">
+      <c r="J10" s="9" t="s">
         <v>23</v>
       </c>
     </row>
@@ -2788,7 +2789,7 @@
       <c r="J14" s="1"/>
     </row>
     <row r="15" spans="1:15">
-      <c r="L15" s="11"/>
+      <c r="L15" s="10"/>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
@@ -2802,7 +2803,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{718B6DC5-6D40-48B9-9720-0693B947ED0C}">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="Y24" sqref="Y24"/>
     </sheetView>
   </sheetViews>
@@ -2817,19 +2818,19 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B1" t="s">
         <v>45</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>46</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>47</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>48</v>
-      </c>
-      <c r="E1" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:5">

</xml_diff>